<commit_message>
another make you kingdom pic
</commit_message>
<xml_diff>
--- a/meikyuu-kingdom/checklist.xlsx
+++ b/meikyuu-kingdom/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/meikyuu-kingdom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05BC5172-8778-6842-8422-75E14B5F0B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D50AF44-B85D-6B45-8E8C-8F3F464D7C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="26740" windowHeight="15780" xr2:uid="{A3DAF738-D573-0A4B-A3EC-667E97A5D603}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="101">
   <si>
     <t>year</t>
   </si>
@@ -328,6 +328,15 @@
   </si>
   <si>
     <t>frontier_kingdom_and_cheese_forest.jpg</t>
+  </si>
+  <si>
+    <t>大冒険ブック 旅する王国と無名階域</t>
+  </si>
+  <si>
+    <t>Great Adventure Book: Traveling Kingdom and Anonymous Floors</t>
+  </si>
+  <si>
+    <t>great_adventure_book.jpg</t>
   </si>
 </sst>
 </file>
@@ -694,16 +703,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9C575D-DD28-9348-A637-ACBE5E01B1E5}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="57" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="3" max="3" width="53.83203125" customWidth="1"/>
     <col min="4" max="4" width="30.33203125" customWidth="1"/>
     <col min="5" max="5" width="33.6640625" customWidth="1"/>
   </cols>
@@ -1320,6 +1329,26 @@
       </c>
       <c r="F31" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2021</v>
+      </c>
+      <c r="B32" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" t="s">
+        <v>100</v>
+      </c>
+      <c r="F32" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dates for make you kingdom
</commit_message>
<xml_diff>
--- a/meikyuu-kingdom/checklist.xlsx
+++ b/meikyuu-kingdom/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/meikyuu-kingdom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D50AF44-B85D-6B45-8E8C-8F3F464D7C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{10AE75F1-1131-464D-9FEE-EFEE37C535D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="26740" windowHeight="15780" xr2:uid="{A3DAF738-D573-0A4B-A3EC-667E97A5D603}"/>
   </bookViews>
@@ -706,7 +706,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -978,6 +978,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2007</v>
+      </c>
       <c r="B14" t="s">
         <v>75</v>
       </c>
@@ -1155,6 +1158,9 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2011</v>
+      </c>
       <c r="B23" t="s">
         <v>93</v>
       </c>

</xml_diff>